<commit_message>
Comienzo del ejercicio 3
</commit_message>
<xml_diff>
--- a/practica-SistemasNumericos/Practica 1 - Sistemas Numericos.xlsx
+++ b/practica-SistemasNumericos/Practica 1 - Sistemas Numericos.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\Materias\Primer Año\Segundo Cuatrimestre\Arquitectura de Computadoras I\Logica Digital\Ejercicios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leand\Desktop\workspace\IPS-Practica-Assembly\practica-SistemasNumericos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDFA971-DED3-4743-80CD-7F3AA6E37B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42BC839-FED7-42E2-A44E-A20C1D62AF51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8FFFAB9A-3267-49B9-97BB-6FBD1FE317F3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{8FFFAB9A-3267-49B9-97BB-6FBD1FE317F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Ej1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ej2" sheetId="2" r:id="rId2"/>
+    <sheet name="Ej3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -23,9 +25,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -35,14 +35,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>Decimal</t>
   </si>
@@ -72,13 +72,85 @@
   </si>
   <si>
     <t>Parte Flotante</t>
+  </si>
+  <si>
+    <t>Base 10</t>
+  </si>
+  <si>
+    <t>VAS</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>010111</t>
+  </si>
+  <si>
+    <t>0101111</t>
+  </si>
+  <si>
+    <t>11110</t>
+  </si>
+  <si>
+    <t>111011</t>
+  </si>
+  <si>
+    <t>011010101</t>
+  </si>
+  <si>
+    <t>110101</t>
+  </si>
+  <si>
+    <t>10001</t>
+  </si>
+  <si>
+    <t>101010</t>
+  </si>
+  <si>
+    <t>100100</t>
+  </si>
+  <si>
+    <t>10010</t>
+  </si>
+  <si>
+    <t>101011</t>
+  </si>
+  <si>
+    <t>100101</t>
+  </si>
+  <si>
+    <t>Exceso</t>
+  </si>
+  <si>
+    <t>110111</t>
+  </si>
+  <si>
+    <t>1101111</t>
+  </si>
+  <si>
+    <t>00010</t>
+  </si>
+  <si>
+    <t>001011</t>
+  </si>
+  <si>
+    <t>000101</t>
+  </si>
+  <si>
+    <t>111010101</t>
+  </si>
+  <si>
+    <t>Nuer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,6 +164,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="TimesNewRomanPSMT"/>
     </font>
   </fonts>
   <fills count="4">
@@ -258,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -277,15 +360,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -295,7 +369,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -322,17 +405,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -352,7 +438,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -650,11 +736,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29135B90-0CAE-44F4-A562-E101AA2D558F}">
   <dimension ref="A1:AC56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="6" max="6" width="12.140625" customWidth="1"/>
     <col min="7" max="7" width="13.140625" customWidth="1"/>
@@ -665,30 +751,30 @@
     <col min="29" max="29" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:29">
+      <c r="A1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="35" t="s">
+      <c r="C1" s="26"/>
+      <c r="D1" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="32"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="36"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="34"/>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="37">
+      <c r="E1" s="29"/>
+      <c r="F1" s="26"/>
+    </row>
+    <row r="2" spans="1:29">
+      <c r="A2" s="30"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="28"/>
+    </row>
+    <row r="3" spans="1:29">
+      <c r="A3" s="20">
         <v>25.75</v>
       </c>
       <c r="B3" s="1">
@@ -707,10 +793,10 @@
         <f>INT(E3)</f>
         <v>1</v>
       </c>
-      <c r="I3" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="J3" s="25" t="s">
+      <c r="I3" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="16" t="s">
         <v>1</v>
       </c>
       <c r="K3" s="14">
@@ -785,8 +871,8 @@
         <v>262144</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="38"/>
+    <row r="4" spans="1:29">
+      <c r="A4" s="21"/>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B7" si="1">QUOTIENT(B3,2)</f>
         <v>12</v>
@@ -806,91 +892,91 @@
         <f>INT(E4)</f>
         <v>1</v>
       </c>
-      <c r="I4" s="29">
-        <v>25.75</v>
-      </c>
-      <c r="J4" s="30" t="str">
+      <c r="I4" s="23">
+        <v>14</v>
+      </c>
+      <c r="J4" s="24" t="str">
         <f>_xlfn.TEXTJOIN(,TRUE,K6:AB6)&amp;IF(K7&lt;&gt;0,"."&amp;_xlfn.TEXTJOIN(,TRUE,L8:AB8),"")</f>
-        <v>11001.11</v>
-      </c>
-      <c r="K4" s="27">
+        <v>1110</v>
+      </c>
+      <c r="K4" s="18">
         <f>INT(I4)</f>
-        <v>25</v>
-      </c>
-      <c r="L4" s="26">
+        <v>14</v>
+      </c>
+      <c r="L4" s="17">
         <f>IFERROR(IF(QUOTIENT(K4,2)=0,"",QUOTIENT(K4,2)),"")</f>
-        <v>12</v>
-      </c>
-      <c r="M4" s="26">
+        <v>7</v>
+      </c>
+      <c r="M4" s="17">
         <f t="shared" ref="M4:S4" si="2">IFERROR(IF(QUOTIENT(L4,2)=0,"",QUOTIENT(L4,2)),"")</f>
-        <v>6</v>
-      </c>
-      <c r="N4" s="26">
+        <v>3</v>
+      </c>
+      <c r="N4" s="17">
         <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O4" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P4" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="Q4" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="R4" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S4" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="T4" s="17" t="str">
+        <f>IFERROR(IF(QUOTIENT(S4,2)=0,"",QUOTIENT(S4,2)),"")</f>
+        <v/>
+      </c>
+      <c r="U4" s="17" t="str">
+        <f t="shared" ref="U4:V4" si="3">IFERROR(IF(QUOTIENT(T4,2)=0,"",QUOTIENT(T4,2)),"")</f>
+        <v/>
+      </c>
+      <c r="V4" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="W4" s="17" t="str">
+        <f>IFERROR(IF(QUOTIENT(V4,2)=0,"",QUOTIENT(V4,2)),"")</f>
+        <v/>
+      </c>
+      <c r="X4" s="17" t="str">
+        <f t="shared" ref="X4:AB4" si="4">IFERROR(IF(QUOTIENT(W4,2)=0,"",QUOTIENT(W4,2)),"")</f>
+        <v/>
+      </c>
+      <c r="Y4" s="17" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Z4" s="17" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AA4" s="17" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AB4" s="17" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AC4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="26">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="P4" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="Q4" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="R4" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="S4" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="T4" s="26" t="str">
-        <f>IFERROR(IF(QUOTIENT(S4,2)=0,"",QUOTIENT(S4,2)),"")</f>
-        <v/>
-      </c>
-      <c r="U4" s="26" t="str">
-        <f t="shared" ref="U4:V4" si="3">IFERROR(IF(QUOTIENT(T4,2)=0,"",QUOTIENT(T4,2)),"")</f>
-        <v/>
-      </c>
-      <c r="V4" s="26" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="W4" s="26" t="str">
-        <f>IFERROR(IF(QUOTIENT(V4,2)=0,"",QUOTIENT(V4,2)),"")</f>
-        <v/>
-      </c>
-      <c r="X4" s="26" t="str">
-        <f t="shared" ref="X4:AB4" si="4">IFERROR(IF(QUOTIENT(W4,2)=0,"",QUOTIENT(W4,2)),"")</f>
-        <v/>
-      </c>
-      <c r="Y4" s="26" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="Z4" s="26" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="AA4" s="26" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="AB4" s="26" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="AC4" s="37" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A5" s="38"/>
+    </row>
+    <row r="5" spans="1:29">
+      <c r="A5" s="21"/>
       <c r="B5" s="3">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -900,80 +986,80 @@
         <v>0</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="30"/>
-      <c r="L5" s="26">
+      <c r="I5" s="23"/>
+      <c r="J5" s="24"/>
+      <c r="L5" s="17">
         <f t="shared" ref="L5:W5" si="6">IFERROR(IF(K4&gt;1,MOD(K4,2),""),"")</f>
-        <v>1</v>
-      </c>
-      <c r="M5" s="26">
+        <v>0</v>
+      </c>
+      <c r="M5" s="17">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="N5" s="26">
+        <v>1</v>
+      </c>
+      <c r="N5" s="17">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="O5" s="26">
+        <v>1</v>
+      </c>
+      <c r="O5" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="P5" s="26" t="str">
+        <v/>
+      </c>
+      <c r="P5" s="17" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="Q5" s="26" t="str">
+      <c r="Q5" s="17" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="R5" s="26" t="str">
+      <c r="R5" s="17" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="S5" s="26" t="str">
+      <c r="S5" s="17" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="T5" s="26" t="str">
+      <c r="T5" s="17" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="U5" s="26" t="str">
+      <c r="U5" s="17" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="V5" s="26" t="str">
+      <c r="V5" s="17" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="W5" s="26" t="str">
+      <c r="W5" s="17" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="X5" s="26" t="str">
+      <c r="X5" s="17" t="str">
         <f t="shared" ref="X5:AB5" si="7">IFERROR(IF(W4&gt;1,MOD(W4,2),""),"")</f>
         <v/>
       </c>
-      <c r="Y5" s="26" t="str">
+      <c r="Y5" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="Z5" s="26" t="str">
+      <c r="Z5" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="AA5" s="26" t="str">
+      <c r="AA5" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="AB5" s="26" t="str">
+      <c r="AB5" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="AC5" s="38"/>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="38"/>
+      <c r="AC5" s="21"/>
+    </row>
+    <row r="6" spans="1:29">
+      <c r="A6" s="21"/>
       <c r="B6" s="3">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -983,84 +1069,84 @@
         <v>0</v>
       </c>
       <c r="F6" s="4"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="26">
+      <c r="I6" s="23"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="17">
         <f>IF(I4=0,0,1)</f>
         <v>1</v>
       </c>
-      <c r="L6" s="28" cm="1">
+      <c r="L6" s="19" cm="1">
         <f t="array" ref="L6">IF(L5&lt;&gt;"",INDEX($L5:$AB5,,COLUMNS(L5:$AB5)-COUNTIF(L5:$AB5,"")),"")</f>
         <v>1</v>
       </c>
-      <c r="M6" s="28" cm="1">
+      <c r="M6" s="19" cm="1">
         <f t="array" ref="M6">IF(M5&lt;&gt;"",INDEX($L5:$AB5,,COLUMNS(M5:$AB5)-COUNTIF(M5:$AB5,"")),"")</f>
-        <v>0</v>
-      </c>
-      <c r="N6" s="28" cm="1">
+        <v>1</v>
+      </c>
+      <c r="N6" s="19" cm="1">
         <f t="array" ref="N6">IF(N5&lt;&gt;"",INDEX($L5:$AB5,,COLUMNS(N5:$AB5)-COUNTIF(N5:$AB5,"")),"")</f>
         <v>0</v>
       </c>
-      <c r="O6" s="28" cm="1">
+      <c r="O6" s="19" t="str" cm="1">
         <f t="array" ref="O6">IF(O5&lt;&gt;"",INDEX($L5:$AB5,,COLUMNS(O5:$AB5)-COUNTIF(O5:$AB5,"")),"")</f>
-        <v>1</v>
-      </c>
-      <c r="P6" s="28" t="str" cm="1">
+        <v/>
+      </c>
+      <c r="P6" s="19" t="str" cm="1">
         <f t="array" ref="P6">IF(P5&lt;&gt;"",INDEX($L5:$AB5,,COLUMNS(P5:$AB5)-COUNTIF(P5:$AB5,"")),"")</f>
         <v/>
       </c>
-      <c r="Q6" s="28" t="str" cm="1">
+      <c r="Q6" s="19" t="str" cm="1">
         <f t="array" ref="Q6">IF(Q5&lt;&gt;"",INDEX($L5:$AB5,,COLUMNS(Q5:$AB5)-COUNTIF(Q5:$AB5,"")),"")</f>
         <v/>
       </c>
-      <c r="R6" s="28" t="str" cm="1">
+      <c r="R6" s="19" t="str" cm="1">
         <f t="array" ref="R6">IF(R5&lt;&gt;"",INDEX($L5:$AB5,,COLUMNS(R5:$AB5)-COUNTIF(R5:$AB5,"")),"")</f>
         <v/>
       </c>
-      <c r="S6" s="28" t="str" cm="1">
+      <c r="S6" s="19" t="str" cm="1">
         <f t="array" ref="S6">IF(S5&lt;&gt;"",INDEX($L5:$AB5,,COLUMNS(S5:$AB5)-COUNTIF(S5:$AB5,"")),"")</f>
         <v/>
       </c>
-      <c r="T6" s="28" t="str" cm="1">
+      <c r="T6" s="19" t="str" cm="1">
         <f t="array" ref="T6">IF(T5&lt;&gt;"",INDEX($L5:$AB5,,COLUMNS(T5:$AB5)-COUNTIF(T5:$AB5,"")),"")</f>
         <v/>
       </c>
-      <c r="U6" s="28" t="str" cm="1">
+      <c r="U6" s="19" t="str" cm="1">
         <f t="array" ref="U6">IF(U5&lt;&gt;"",INDEX($L5:$AB5,,COLUMNS(U5:$AB5)-COUNTIF(U5:$AB5,"")),"")</f>
         <v/>
       </c>
-      <c r="V6" s="28" t="str" cm="1">
+      <c r="V6" s="19" t="str" cm="1">
         <f t="array" ref="V6">IF(V5&lt;&gt;"",INDEX($L5:$AB5,,COLUMNS(V5:$AB5)-COUNTIF(V5:$AB5,"")),"")</f>
         <v/>
       </c>
-      <c r="W6" s="28" t="str" cm="1">
+      <c r="W6" s="19" t="str" cm="1">
         <f t="array" ref="W6">IF(W5&lt;&gt;"",INDEX($L5:$AB5,,COLUMNS(W5:$AB5)-COUNTIF(W5:$AB5,"")),"")</f>
         <v/>
       </c>
-      <c r="X6" s="28" t="str" cm="1">
+      <c r="X6" s="19" t="str" cm="1">
         <f t="array" ref="X6">IF(X5&lt;&gt;"",INDEX($L5:$AB5,,COLUMNS(X5:$AB5)-COUNTIF(X5:$AB5,"")),"")</f>
         <v/>
       </c>
-      <c r="Y6" s="28" t="str" cm="1">
+      <c r="Y6" s="19" t="str" cm="1">
         <f t="array" ref="Y6">IF(Y5&lt;&gt;"",INDEX($L5:$AB5,,COLUMNS(Y5:$AB5)-COUNTIF(Y5:$AB5,"")),"")</f>
         <v/>
       </c>
-      <c r="Z6" s="28" t="str" cm="1">
+      <c r="Z6" s="19" t="str" cm="1">
         <f t="array" ref="Z6">IF(Z5&lt;&gt;"",INDEX($L5:$AB5,,COLUMNS(Z5:$AB5)-COUNTIF(Z5:$AB5,"")),"")</f>
         <v/>
       </c>
-      <c r="AA6" s="28" t="str" cm="1">
+      <c r="AA6" s="19" t="str" cm="1">
         <f t="array" ref="AA6">IF(AA5&lt;&gt;"",INDEX($L5:$AB5,,COLUMNS(AA5:$AB5)-COUNTIF(AA5:$AB5,"")),"")</f>
         <v/>
       </c>
-      <c r="AB6" s="28" t="str" cm="1">
+      <c r="AB6" s="19" t="str" cm="1">
         <f t="array" ref="AB6">IF(AB5&lt;&gt;"",INDEX($L5:$AB5,,COLUMNS(AB5:$AB5)-COUNTIF(AB5:$AB5,"")),"")</f>
         <v/>
       </c>
-      <c r="AC6" s="39"/>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="39"/>
+      <c r="AC6" s="22"/>
+    </row>
+    <row r="7" spans="1:29">
+      <c r="A7" s="22"/>
       <c r="B7" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -1072,86 +1158,86 @@
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="7"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="26">
+      <c r="I7" s="23"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="17">
         <f>+MOD(I4,K4)</f>
-        <v>0.75</v>
-      </c>
-      <c r="L7" s="26">
+        <v>0</v>
+      </c>
+      <c r="L7" s="17" t="str">
         <f>IFERROR(IF(OR(K7=1,K7=0),"",(K7-K8)*2),"")</f>
-        <v>1.5</v>
-      </c>
-      <c r="M7" s="26">
+        <v/>
+      </c>
+      <c r="M7" s="17" t="str">
         <f t="shared" ref="M7:V7" si="8">IFERROR(IF(L7=1,"",(L7-L8)*2),"")</f>
-        <v>1</v>
-      </c>
-      <c r="N7" s="26" t="str">
+        <v/>
+      </c>
+      <c r="N7" s="17" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="O7" s="26" t="str">
+      <c r="O7" s="17" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="P7" s="26" t="str">
+      <c r="P7" s="17" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="Q7" s="26" t="str">
+      <c r="Q7" s="17" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="R7" s="26" t="str">
+      <c r="R7" s="17" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="S7" s="26" t="str">
+      <c r="S7" s="17" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="T7" s="26" t="str">
+      <c r="T7" s="17" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="U7" s="26" t="str">
+      <c r="U7" s="17" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="V7" s="26" t="str">
+      <c r="V7" s="17" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="W7" s="26" t="str">
+      <c r="W7" s="17" t="str">
         <f>IFERROR(IF(V7=1,"",(V7-V8)*2),"")</f>
         <v/>
       </c>
-      <c r="X7" s="26" t="str">
+      <c r="X7" s="17" t="str">
         <f t="shared" ref="X7:AB7" si="9">IFERROR(IF(W7=1,"",(W7-W8)*2),"")</f>
         <v/>
       </c>
-      <c r="Y7" s="26" t="str">
+      <c r="Y7" s="17" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="Z7" s="26" t="str">
+      <c r="Z7" s="17" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="AA7" s="26" t="str">
+      <c r="AA7" s="17" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="AB7" s="26" t="str">
+      <c r="AB7" s="17" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="AC7" s="37" t="s">
+      <c r="AC7" s="20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A8" s="37">
+    <row r="8" spans="1:29">
+      <c r="A8" s="20">
         <v>14.16</v>
       </c>
       <c r="B8" s="1">
@@ -1169,81 +1255,81 @@
         <f t="shared" ref="F8:F37" si="10">INT(E8)</f>
         <v>0</v>
       </c>
-      <c r="I8" s="29"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26">
+      <c r="I8" s="23"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17" t="str">
         <f t="shared" ref="L8:M8" si="11">IF(L7="","",INT(L7))</f>
-        <v>1</v>
-      </c>
-      <c r="M8" s="26">
+        <v/>
+      </c>
+      <c r="M8" s="17" t="str">
         <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="N8" s="26" t="str">
+        <v/>
+      </c>
+      <c r="N8" s="17" t="str">
         <f>IF(N7="","",INT(N7))</f>
         <v/>
       </c>
-      <c r="O8" s="26" t="str">
+      <c r="O8" s="17" t="str">
         <f t="shared" ref="O8:W8" si="12">IF(O7="","",INT(O7))</f>
         <v/>
       </c>
-      <c r="P8" s="26" t="str">
+      <c r="P8" s="17" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="Q8" s="26" t="str">
+      <c r="Q8" s="17" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="R8" s="26" t="str">
+      <c r="R8" s="17" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="S8" s="26" t="str">
+      <c r="S8" s="17" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="T8" s="26" t="str">
+      <c r="T8" s="17" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="U8" s="26" t="str">
+      <c r="U8" s="17" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="V8" s="26" t="str">
+      <c r="V8" s="17" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="W8" s="26" t="str">
+      <c r="W8" s="17" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="X8" s="26" t="str">
+      <c r="X8" s="17" t="str">
         <f t="shared" ref="X8" si="13">IF(X7="","",INT(X7))</f>
         <v/>
       </c>
-      <c r="Y8" s="26" t="str">
+      <c r="Y8" s="17" t="str">
         <f t="shared" ref="Y8" si="14">IF(Y7="","",INT(Y7))</f>
         <v/>
       </c>
-      <c r="Z8" s="26" t="str">
+      <c r="Z8" s="17" t="str">
         <f t="shared" ref="Z8" si="15">IF(Z7="","",INT(Z7))</f>
         <v/>
       </c>
-      <c r="AA8" s="26" t="str">
+      <c r="AA8" s="17" t="str">
         <f t="shared" ref="AA8" si="16">IF(AA7="","",INT(AA7))</f>
         <v/>
       </c>
-      <c r="AB8" s="26" t="str">
+      <c r="AB8" s="17" t="str">
         <f t="shared" ref="AB8" si="17">IF(AB7="","",INT(AB7))</f>
         <v/>
       </c>
-      <c r="AC8" s="39"/>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A9" s="38"/>
+      <c r="AC8" s="22"/>
+    </row>
+    <row r="9" spans="1:29">
+      <c r="A9" s="21"/>
       <c r="B9">
         <f t="shared" ref="B9:B11" si="18">QUOTIENT(B8,2)</f>
         <v>7</v>
@@ -1264,8 +1350,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
+    <row r="10" spans="1:29">
+      <c r="A10" s="21"/>
       <c r="B10">
         <f t="shared" si="18"/>
         <v>3</v>
@@ -1286,8 +1372,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="38"/>
+    <row r="11" spans="1:29">
+      <c r="A11" s="21"/>
       <c r="B11" s="15">
         <f t="shared" si="18"/>
         <v>1</v>
@@ -1308,8 +1394,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A12" s="38"/>
+    <row r="12" spans="1:29">
+      <c r="A12" s="21"/>
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
       <c r="D12">
@@ -1324,8 +1410,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A13" s="38"/>
+    <row r="13" spans="1:29">
+      <c r="A13" s="21"/>
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
       <c r="D13">
@@ -1340,8 +1426,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A14" s="38"/>
+    <row r="14" spans="1:29">
+      <c r="A14" s="21"/>
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
       <c r="D14">
@@ -1356,8 +1442,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A15" s="38"/>
+    <row r="15" spans="1:29">
+      <c r="A15" s="21"/>
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
       <c r="D15">
@@ -1372,8 +1458,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A16" s="38"/>
+    <row r="16" spans="1:29">
+      <c r="A16" s="21"/>
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
       <c r="D16">
@@ -1388,8 +1474,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="38"/>
+    <row r="17" spans="1:6">
+      <c r="A17" s="21"/>
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
       <c r="D17">
@@ -1404,8 +1490,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="38"/>
+    <row r="18" spans="1:6">
+      <c r="A18" s="21"/>
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
       <c r="D18">
@@ -1420,8 +1506,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="38"/>
+    <row r="19" spans="1:6">
+      <c r="A19" s="21"/>
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
       <c r="D19">
@@ -1436,8 +1522,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="38"/>
+    <row r="20" spans="1:6">
+      <c r="A20" s="21"/>
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
       <c r="D20">
@@ -1452,8 +1538,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="38"/>
+    <row r="21" spans="1:6">
+      <c r="A21" s="21"/>
       <c r="B21" s="3"/>
       <c r="C21" s="4"/>
       <c r="D21">
@@ -1468,8 +1554,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="38"/>
+    <row r="22" spans="1:6">
+      <c r="A22" s="21"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
       <c r="D22">
@@ -1484,8 +1570,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="38"/>
+    <row r="23" spans="1:6">
+      <c r="A23" s="21"/>
       <c r="B23" s="3"/>
       <c r="C23" s="4"/>
       <c r="D23">
@@ -1500,8 +1586,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="38"/>
+    <row r="24" spans="1:6">
+      <c r="A24" s="21"/>
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
       <c r="D24">
@@ -1516,8 +1602,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="38"/>
+    <row r="25" spans="1:6">
+      <c r="A25" s="21"/>
       <c r="B25" s="3"/>
       <c r="C25" s="4"/>
       <c r="D25">
@@ -1532,8 +1618,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="38"/>
+    <row r="26" spans="1:6">
+      <c r="A26" s="21"/>
       <c r="B26" s="3"/>
       <c r="C26" s="4"/>
       <c r="D26">
@@ -1548,8 +1634,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="38"/>
+    <row r="27" spans="1:6">
+      <c r="A27" s="21"/>
       <c r="B27" s="3"/>
       <c r="C27" s="4"/>
       <c r="D27">
@@ -1564,14 +1650,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="39"/>
+    <row r="28" spans="1:6">
+      <c r="A28" s="22"/>
       <c r="B28" s="5"/>
       <c r="C28" s="7"/>
-      <c r="D28" s="18">
+      <c r="D28">
         <v>0.16</v>
       </c>
-      <c r="E28" s="18">
+      <c r="E28">
         <f t="shared" si="19"/>
         <v>0.32</v>
       </c>
@@ -1580,8 +1666,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="37">
+    <row r="29" spans="1:6">
+      <c r="A29" s="20">
         <v>7.9</v>
       </c>
       <c r="B29" s="1">
@@ -1600,8 +1686,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="38"/>
+    <row r="30" spans="1:6">
+      <c r="A30" s="21"/>
       <c r="B30">
         <f t="shared" ref="B30:B31" si="20">QUOTIENT(B29,2)</f>
         <v>3</v>
@@ -1613,7 +1699,7 @@
       <c r="D30" s="3">
         <v>0.8</v>
       </c>
-      <c r="E30" s="18">
+      <c r="E30">
         <f t="shared" si="19"/>
         <v>1.6</v>
       </c>
@@ -1622,8 +1708,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="38"/>
+    <row r="31" spans="1:6">
+      <c r="A31" s="21"/>
       <c r="B31" s="15">
         <f t="shared" si="20"/>
         <v>1</v>
@@ -1635,7 +1721,7 @@
       <c r="D31" s="3">
         <v>0.6</v>
       </c>
-      <c r="E31" s="18">
+      <c r="E31">
         <f t="shared" si="19"/>
         <v>1.2</v>
       </c>
@@ -1644,14 +1730,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="38"/>
+    <row r="32" spans="1:6">
+      <c r="A32" s="21"/>
       <c r="B32" s="3"/>
       <c r="C32" s="4"/>
       <c r="D32" s="3">
         <v>0.2</v>
       </c>
-      <c r="E32" s="18">
+      <c r="E32">
         <f t="shared" si="19"/>
         <v>0.4</v>
       </c>
@@ -1660,14 +1746,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="38"/>
+    <row r="33" spans="1:6">
+      <c r="A33" s="21"/>
       <c r="B33" s="3"/>
       <c r="C33" s="4"/>
       <c r="D33" s="3">
         <v>0.4</v>
       </c>
-      <c r="E33" s="18">
+      <c r="E33">
         <f t="shared" si="19"/>
         <v>0.8</v>
       </c>
@@ -1676,14 +1762,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="38"/>
+    <row r="34" spans="1:6">
+      <c r="A34" s="21"/>
       <c r="B34" s="3"/>
       <c r="C34" s="4"/>
       <c r="D34" s="3">
         <v>0.8</v>
       </c>
-      <c r="E34" s="18">
+      <c r="E34">
         <f t="shared" si="19"/>
         <v>1.6</v>
       </c>
@@ -1692,8 +1778,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="39"/>
+    <row r="35" spans="1:6">
+      <c r="A35" s="22"/>
       <c r="B35" s="5"/>
       <c r="C35" s="7"/>
       <c r="D35" s="5">
@@ -1708,18 +1794,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="37">
+    <row r="36" spans="1:6">
+      <c r="A36" s="20">
         <v>48.25</v>
       </c>
       <c r="B36" s="1">
         <v>48</v>
       </c>
       <c r="C36" s="8"/>
-      <c r="D36" s="19">
+      <c r="D36" s="1">
         <v>0.25</v>
       </c>
-      <c r="E36" s="20">
+      <c r="E36" s="2">
         <f t="shared" si="19"/>
         <v>0.5</v>
       </c>
@@ -1728,8 +1814,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="38"/>
+    <row r="37" spans="1:6">
+      <c r="A37" s="21"/>
       <c r="B37" s="3">
         <f>QUOTIENT(B36,2)</f>
         <v>24</v>
@@ -1741,7 +1827,7 @@
       <c r="D37" s="3">
         <v>0.5</v>
       </c>
-      <c r="E37" s="17">
+      <c r="E37">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
@@ -1750,8 +1836,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="38"/>
+    <row r="38" spans="1:6">
+      <c r="A38" s="21"/>
       <c r="B38" s="3">
         <f t="shared" ref="B38:B41" si="23">QUOTIENT(B37,2)</f>
         <v>12</v>
@@ -1761,11 +1847,10 @@
         <v>0</v>
       </c>
       <c r="D38" s="3"/>
-      <c r="E38" s="18"/>
       <c r="F38" s="9"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="38"/>
+    <row r="39" spans="1:6">
+      <c r="A39" s="21"/>
       <c r="B39" s="3">
         <f t="shared" si="23"/>
         <v>6</v>
@@ -1775,11 +1860,10 @@
         <v>0</v>
       </c>
       <c r="D39" s="3"/>
-      <c r="E39" s="18"/>
       <c r="F39" s="9"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="38"/>
+    <row r="40" spans="1:6">
+      <c r="A40" s="21"/>
       <c r="B40" s="3">
         <f t="shared" si="23"/>
         <v>3</v>
@@ -1789,11 +1873,10 @@
         <v>0</v>
       </c>
       <c r="D40" s="3"/>
-      <c r="E40" s="18"/>
       <c r="F40" s="9"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="39"/>
+    <row r="41" spans="1:6">
+      <c r="A41" s="22"/>
       <c r="B41" s="11">
         <f t="shared" si="23"/>
         <v>1</v>
@@ -1806,18 +1889,18 @@
       <c r="E41" s="6"/>
       <c r="F41" s="10"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="37">
+    <row r="42" spans="1:6">
+      <c r="A42" s="20">
         <v>23.125</v>
       </c>
       <c r="B42" s="1">
         <v>23</v>
       </c>
       <c r="C42" s="8"/>
-      <c r="D42" s="19">
+      <c r="D42" s="1">
         <v>0.125</v>
       </c>
-      <c r="E42" s="20">
+      <c r="E42" s="2">
         <f t="shared" ref="E42:E44" si="24">D42*2</f>
         <v>0.25</v>
       </c>
@@ -1826,8 +1909,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="38"/>
+    <row r="43" spans="1:6">
+      <c r="A43" s="21"/>
       <c r="B43" s="3">
         <f>QUOTIENT(B42,2)</f>
         <v>11</v>
@@ -1839,7 +1922,7 @@
       <c r="D43" s="3">
         <v>0.25</v>
       </c>
-      <c r="E43" s="17">
+      <c r="E43">
         <f t="shared" si="24"/>
         <v>0.5</v>
       </c>
@@ -1848,8 +1931,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="38"/>
+    <row r="44" spans="1:6">
+      <c r="A44" s="21"/>
       <c r="B44" s="3">
         <f>QUOTIENT(B43,2)</f>
         <v>5</v>
@@ -1861,7 +1944,7 @@
       <c r="D44" s="3">
         <v>0.5</v>
       </c>
-      <c r="E44" s="17">
+      <c r="E44">
         <f t="shared" si="24"/>
         <v>1</v>
       </c>
@@ -1870,8 +1953,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="38"/>
+    <row r="45" spans="1:6">
+      <c r="A45" s="21"/>
       <c r="B45" s="3">
         <f>QUOTIENT(B44,2)</f>
         <v>2</v>
@@ -1881,11 +1964,10 @@
         <v>1</v>
       </c>
       <c r="D45" s="3"/>
-      <c r="E45" s="18"/>
       <c r="F45" s="9"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="39"/>
+    <row r="46" spans="1:6">
+      <c r="A46" s="22"/>
       <c r="B46" s="13">
         <f>QUOTIENT(B45,2)</f>
         <v>1</v>
@@ -1898,18 +1980,18 @@
       <c r="E46" s="6"/>
       <c r="F46" s="10"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="37">
+    <row r="47" spans="1:6">
+      <c r="A47" s="20">
         <v>51.7</v>
       </c>
       <c r="B47" s="1">
         <v>51</v>
       </c>
       <c r="C47" s="8"/>
-      <c r="D47" s="19">
+      <c r="D47" s="1">
         <v>0.7</v>
       </c>
-      <c r="E47" s="20">
+      <c r="E47" s="2">
         <f>D47*2</f>
         <v>1.4</v>
       </c>
@@ -1918,8 +2000,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="38"/>
+    <row r="48" spans="1:6">
+      <c r="A48" s="21"/>
       <c r="B48" s="3">
         <f>QUOTIENT(B47,2)</f>
         <v>25</v>
@@ -1931,7 +2013,7 @@
       <c r="D48" s="3">
         <v>0.4</v>
       </c>
-      <c r="E48" s="17">
+      <c r="E48">
         <f t="shared" ref="E48:E56" si="27">D48*2</f>
         <v>0.8</v>
       </c>
@@ -1940,8 +2022,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="38"/>
+    <row r="49" spans="1:6">
+      <c r="A49" s="21"/>
       <c r="B49" s="3">
         <f>QUOTIENT(B48,2)</f>
         <v>12</v>
@@ -1953,7 +2035,7 @@
       <c r="D49" s="3">
         <v>0.8</v>
       </c>
-      <c r="E49" s="17">
+      <c r="E49">
         <f t="shared" si="27"/>
         <v>1.6</v>
       </c>
@@ -1962,8 +2044,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="38"/>
+    <row r="50" spans="1:6">
+      <c r="A50" s="21"/>
       <c r="B50" s="3">
         <f>QUOTIENT(B49,2)</f>
         <v>6</v>
@@ -1975,7 +2057,7 @@
       <c r="D50" s="3">
         <v>0.6</v>
       </c>
-      <c r="E50" s="17">
+      <c r="E50">
         <f t="shared" si="27"/>
         <v>1.2</v>
       </c>
@@ -1984,8 +2066,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="38"/>
+    <row r="51" spans="1:6">
+      <c r="A51" s="21"/>
       <c r="B51" s="3">
         <f>QUOTIENT(B50,2)</f>
         <v>3</v>
@@ -1997,7 +2079,7 @@
       <c r="D51" s="3">
         <v>0.2</v>
       </c>
-      <c r="E51" s="17">
+      <c r="E51">
         <f t="shared" si="27"/>
         <v>0.4</v>
       </c>
@@ -2006,8 +2088,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="38"/>
+    <row r="52" spans="1:6">
+      <c r="A52" s="21"/>
       <c r="B52" s="13">
         <f>QUOTIENT(B51,2)</f>
         <v>1</v>
@@ -2019,7 +2101,7 @@
       <c r="D52" s="3">
         <v>0.4</v>
       </c>
-      <c r="E52" s="17">
+      <c r="E52">
         <f t="shared" si="27"/>
         <v>0.8</v>
       </c>
@@ -2028,72 +2110,76 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="38"/>
+    <row r="53" spans="1:6">
+      <c r="A53" s="21"/>
       <c r="B53" s="3"/>
       <c r="C53" s="4"/>
-      <c r="D53" s="16">
+      <c r="D53" s="3">
         <v>0.8</v>
       </c>
-      <c r="E53" s="17">
+      <c r="E53">
         <f t="shared" si="27"/>
         <v>1.6</v>
       </c>
-      <c r="F53" s="21">
+      <c r="F53" s="9">
         <f t="shared" si="26"/>
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="38"/>
+    <row r="54" spans="1:6">
+      <c r="A54" s="21"/>
       <c r="B54" s="3"/>
       <c r="C54" s="4"/>
-      <c r="D54" s="16">
+      <c r="D54" s="3">
         <v>0.6</v>
       </c>
-      <c r="E54" s="17">
+      <c r="E54">
         <f t="shared" si="27"/>
         <v>1.2</v>
       </c>
-      <c r="F54" s="21">
+      <c r="F54" s="9">
         <f t="shared" si="26"/>
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="38"/>
+    <row r="55" spans="1:6">
+      <c r="A55" s="21"/>
       <c r="B55" s="3"/>
       <c r="C55" s="4"/>
-      <c r="D55" s="16">
+      <c r="D55" s="3">
         <v>0.2</v>
       </c>
-      <c r="E55" s="17">
+      <c r="E55">
         <f t="shared" si="27"/>
         <v>0.4</v>
       </c>
-      <c r="F55" s="21">
+      <c r="F55" s="9">
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="39"/>
+    <row r="56" spans="1:6">
+      <c r="A56" s="22"/>
       <c r="B56" s="5"/>
       <c r="C56" s="7"/>
-      <c r="D56" s="22">
+      <c r="D56" s="5">
         <v>0.4</v>
       </c>
-      <c r="E56" s="23">
+      <c r="E56" s="6">
         <f t="shared" si="27"/>
         <v>0.8</v>
       </c>
-      <c r="F56" s="24">
+      <c r="F56" s="10">
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:F2"/>
+    <mergeCell ref="A42:A46"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="AC4:AC6"/>
     <mergeCell ref="AC7:AC8"/>
     <mergeCell ref="A47:A56"/>
@@ -2103,10 +2189,6 @@
     <mergeCell ref="A8:A28"/>
     <mergeCell ref="I4:I8"/>
     <mergeCell ref="J4:J8"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="D1:F2"/>
-    <mergeCell ref="A42:A46"/>
-    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB3" xr:uid="{9E8DEBF0-81D7-470F-B5CE-A40A8938D778}">
@@ -2116,4 +2198,165 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51FAEC6C-1B1D-4A7B-9F1F-975F14C39F83}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="32">
+        <v>23</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="32">
+        <v>47</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="32">
+        <v>-14</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="32">
+        <v>-21</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="32">
+        <v>-27</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="32">
+        <v>213</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B6:C6 B2:C3 B7:C7 B4:C4 B5:C5 D7 D2 D3 D4 D5 D6 E2:E7" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493D1E45-CE79-430B-B487-A22C8C16D2D9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75">
+      <c r="A1" s="35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Resolucion ejercicio 2 de Sistemas Numericos
</commit_message>
<xml_diff>
--- a/practica-SistemasNumericos/Practica 1 - Sistemas Numericos.xlsx
+++ b/practica-SistemasNumericos/Practica 1 - Sistemas Numericos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leand\Desktop\workspace\IPS-Practica-Assembly\practica-SistemasNumericos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42BC839-FED7-42E2-A44E-A20C1D62AF51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E49A433-85C0-4E1A-90CC-ECFCF511BB5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{8FFFAB9A-3267-49B9-97BB-6FBD1FE317F3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{8FFFAB9A-3267-49B9-97BB-6FBD1FE317F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Ej1" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
   <si>
     <t>Decimal</t>
   </si>
@@ -74,54 +74,15 @@
     <t>Parte Flotante</t>
   </si>
   <si>
-    <t>Base 10</t>
-  </si>
-  <si>
-    <t>VAS</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
     <t>010111</t>
   </si>
   <si>
     <t>0101111</t>
   </si>
   <si>
-    <t>11110</t>
-  </si>
-  <si>
-    <t>111011</t>
-  </si>
-  <si>
     <t>011010101</t>
   </si>
   <si>
-    <t>110101</t>
-  </si>
-  <si>
-    <t>10001</t>
-  </si>
-  <si>
-    <t>101010</t>
-  </si>
-  <si>
-    <t>100100</t>
-  </si>
-  <si>
-    <t>10010</t>
-  </si>
-  <si>
-    <t>101011</t>
-  </si>
-  <si>
-    <t>100101</t>
-  </si>
-  <si>
     <t>Exceso</t>
   </si>
   <si>
@@ -131,26 +92,143 @@
     <t>1101111</t>
   </si>
   <si>
-    <t>00010</t>
-  </si>
-  <si>
-    <t>001011</t>
-  </si>
-  <si>
-    <t>000101</t>
-  </si>
-  <si>
     <t>111010101</t>
   </si>
   <si>
-    <t>Nuer</t>
+    <t>Valor Absoluto y Signo</t>
+  </si>
+  <si>
+    <t>Complemento a 1</t>
+  </si>
+  <si>
+    <t>Complemento a 2</t>
+  </si>
+  <si>
+    <t>010010</t>
+  </si>
+  <si>
+    <t>0101011</t>
+  </si>
+  <si>
+    <t>0100101</t>
+  </si>
+  <si>
+    <t>-1.010 * 2^-10</t>
+  </si>
+  <si>
+    <t>Signo: 1</t>
+  </si>
+  <si>
+    <t>Exponente: 127 - 10 = 117 = 01110101</t>
+  </si>
+  <si>
+    <t>Mantisa normalizada: 010</t>
+  </si>
+  <si>
+    <t>1 01110101 01000000000000000000000</t>
+  </si>
+  <si>
+    <t>Signo: 0</t>
+  </si>
+  <si>
+    <t>Mantisa normalizada: 001</t>
+  </si>
+  <si>
+    <t>0.001 * 2^-4</t>
+  </si>
+  <si>
+    <t>Exponente: 127 - 4 = 123 = 01111011</t>
+  </si>
+  <si>
+    <t>0 01111011 00100000000000000000000</t>
+  </si>
+  <si>
+    <t>1 * 2^-130</t>
+  </si>
+  <si>
+    <t>Exponente: -126 = 00000000</t>
+  </si>
+  <si>
+    <t>Mantisa: 0</t>
+  </si>
+  <si>
+    <t>0 00000000 00010000000000000000000</t>
+  </si>
+  <si>
+    <t>0 11101011 0100…</t>
+  </si>
+  <si>
+    <t>Signo: +</t>
+  </si>
+  <si>
+    <t>Numero: 1.01</t>
+  </si>
+  <si>
+    <t>Exponente: 11101011 -&gt; Exceso 127 -&gt; 235 - 127 = 108</t>
+  </si>
+  <si>
+    <t>1.01 * 2^108</t>
+  </si>
+  <si>
+    <t>Signo: -</t>
+  </si>
+  <si>
+    <t>1 00000000 0101…</t>
+  </si>
+  <si>
+    <t>Numero: 1.0101</t>
+  </si>
+  <si>
+    <t>Exponente: 00000000 -&gt; Exponente 0 y mantisa &lt;&gt; 0 -&gt; -126</t>
+  </si>
+  <si>
+    <t>1.0101 * 2^-126</t>
+  </si>
+  <si>
+    <t>0 11111111 1010…</t>
+  </si>
+  <si>
+    <t>Exponente: 11111111</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>-Infinito</t>
+  </si>
+  <si>
+    <t>1 11111111 00000000000000000000000</t>
+  </si>
+  <si>
+    <t>Mantisa: 01</t>
+  </si>
+  <si>
+    <t>0 11111111 01000000000000000000000</t>
+  </si>
+  <si>
+    <t>122 * 10^3</t>
+  </si>
+  <si>
+    <t>01111010 * 2^3</t>
+  </si>
+  <si>
+    <t>1.111010 * 2^6</t>
+  </si>
+  <si>
+    <t>Exponente: 127 - 6 = 121 = 01111001</t>
+  </si>
+  <si>
+    <t>Mantisa: 111010</t>
+  </si>
+  <si>
+    <t>0 01111001 11101000000000000000000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,9 +250,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="TimesNewRomanPSMT"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -341,7 +421,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -372,21 +452,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -405,21 +470,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -737,10 +812,10 @@
   <dimension ref="A1:AC56"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="12.140625" customWidth="1"/>
     <col min="7" max="7" width="13.140625" customWidth="1"/>
@@ -751,30 +826,30 @@
     <col min="29" max="29" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
-      <c r="A1" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="25" t="s">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="29" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="29"/>
-      <c r="F1" s="26"/>
-    </row>
-    <row r="2" spans="1:29">
-      <c r="A2" s="30"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="28"/>
-    </row>
-    <row r="3" spans="1:29">
-      <c r="A3" s="20">
+      <c r="E1" s="24"/>
+      <c r="F1" s="21"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="25"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="23"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="26">
         <v>25.75</v>
       </c>
       <c r="B3" s="1">
@@ -871,8 +946,8 @@
         <v>262144</v>
       </c>
     </row>
-    <row r="4" spans="1:29">
-      <c r="A4" s="21"/>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" s="27"/>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B7" si="1">QUOTIENT(B3,2)</f>
         <v>12</v>
@@ -892,10 +967,10 @@
         <f>INT(E4)</f>
         <v>1</v>
       </c>
-      <c r="I4" s="23">
+      <c r="I4" s="30">
         <v>14</v>
       </c>
-      <c r="J4" s="24" t="str">
+      <c r="J4" s="31" t="str">
         <f>_xlfn.TEXTJOIN(,TRUE,K6:AB6)&amp;IF(K7&lt;&gt;0,"."&amp;_xlfn.TEXTJOIN(,TRUE,L8:AB8),"")</f>
         <v>1110</v>
       </c>
@@ -971,12 +1046,12 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="AC4" s="20" t="s">
+      <c r="AC4" s="26" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:29">
-      <c r="A5" s="21"/>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" s="27"/>
       <c r="B5" s="3">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -986,8 +1061,8 @@
         <v>0</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="24"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="31"/>
       <c r="L5" s="17">
         <f t="shared" ref="L5:W5" si="6">IFERROR(IF(K4&gt;1,MOD(K4,2),""),"")</f>
         <v>0</v>
@@ -1056,10 +1131,10 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="AC5" s="21"/>
-    </row>
-    <row r="6" spans="1:29">
-      <c r="A6" s="21"/>
+      <c r="AC5" s="27"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" s="27"/>
       <c r="B6" s="3">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -1069,8 +1144,8 @@
         <v>0</v>
       </c>
       <c r="F6" s="4"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="24"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="31"/>
       <c r="K6" s="17">
         <f>IF(I4=0,0,1)</f>
         <v>1</v>
@@ -1143,10 +1218,10 @@
         <f t="array" ref="AB6">IF(AB5&lt;&gt;"",INDEX($L5:$AB5,,COLUMNS(AB5:$AB5)-COUNTIF(AB5:$AB5,"")),"")</f>
         <v/>
       </c>
-      <c r="AC6" s="22"/>
-    </row>
-    <row r="7" spans="1:29">
-      <c r="A7" s="22"/>
+      <c r="AC6" s="28"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="28"/>
       <c r="B7" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -1158,8 +1233,8 @@
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="7"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="24"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="31"/>
       <c r="K7" s="17">
         <f>+MOD(I4,K4)</f>
         <v>0</v>
@@ -1232,12 +1307,12 @@
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="AC7" s="20" t="s">
+      <c r="AC7" s="26" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
-      <c r="A8" s="20">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8" s="26">
         <v>14.16</v>
       </c>
       <c r="B8" s="1">
@@ -1255,8 +1330,8 @@
         <f t="shared" ref="F8:F37" si="10">INT(E8)</f>
         <v>0</v>
       </c>
-      <c r="I8" s="23"/>
-      <c r="J8" s="24"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="31"/>
       <c r="K8" s="17"/>
       <c r="L8" s="17" t="str">
         <f t="shared" ref="L8:M8" si="11">IF(L7="","",INT(L7))</f>
@@ -1326,10 +1401,10 @@
         <f t="shared" ref="AB8" si="17">IF(AB7="","",INT(AB7))</f>
         <v/>
       </c>
-      <c r="AC8" s="22"/>
-    </row>
-    <row r="9" spans="1:29">
-      <c r="A9" s="21"/>
+      <c r="AC8" s="28"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
       <c r="B9">
         <f t="shared" ref="B9:B11" si="18">QUOTIENT(B8,2)</f>
         <v>7</v>
@@ -1350,8 +1425,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:29">
-      <c r="A10" s="21"/>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" s="27"/>
       <c r="B10">
         <f t="shared" si="18"/>
         <v>3</v>
@@ -1372,8 +1447,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:29">
-      <c r="A11" s="21"/>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11" s="27"/>
       <c r="B11" s="15">
         <f t="shared" si="18"/>
         <v>1</v>
@@ -1394,8 +1469,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:29">
-      <c r="A12" s="21"/>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A12" s="27"/>
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
       <c r="D12">
@@ -1410,8 +1485,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:29">
-      <c r="A13" s="21"/>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A13" s="27"/>
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
       <c r="D13">
@@ -1426,8 +1501,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:29">
-      <c r="A14" s="21"/>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A14" s="27"/>
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
       <c r="D14">
@@ -1442,8 +1517,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:29">
-      <c r="A15" s="21"/>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A15" s="27"/>
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
       <c r="D15">
@@ -1458,8 +1533,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:29">
-      <c r="A16" s="21"/>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A16" s="27"/>
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
       <c r="D16">
@@ -1474,8 +1549,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="21"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="27"/>
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
       <c r="D17">
@@ -1490,8 +1565,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="21"/>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="27"/>
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
       <c r="D18">
@@ -1506,8 +1581,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="21"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="27"/>
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
       <c r="D19">
@@ -1522,8 +1597,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="21"/>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="27"/>
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
       <c r="D20">
@@ -1538,8 +1613,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="21"/>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="27"/>
       <c r="B21" s="3"/>
       <c r="C21" s="4"/>
       <c r="D21">
@@ -1554,8 +1629,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="21"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="27"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
       <c r="D22">
@@ -1570,8 +1645,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="21"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="27"/>
       <c r="B23" s="3"/>
       <c r="C23" s="4"/>
       <c r="D23">
@@ -1586,8 +1661,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="21"/>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="27"/>
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
       <c r="D24">
@@ -1602,8 +1677,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="21"/>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="27"/>
       <c r="B25" s="3"/>
       <c r="C25" s="4"/>
       <c r="D25">
@@ -1618,8 +1693,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="21"/>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="27"/>
       <c r="B26" s="3"/>
       <c r="C26" s="4"/>
       <c r="D26">
@@ -1634,8 +1709,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="21"/>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="27"/>
       <c r="B27" s="3"/>
       <c r="C27" s="4"/>
       <c r="D27">
@@ -1650,8 +1725,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="22"/>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="28"/>
       <c r="B28" s="5"/>
       <c r="C28" s="7"/>
       <c r="D28">
@@ -1666,8 +1741,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="20">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="26">
         <v>7.9</v>
       </c>
       <c r="B29" s="1">
@@ -1686,8 +1761,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="21"/>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="27"/>
       <c r="B30">
         <f t="shared" ref="B30:B31" si="20">QUOTIENT(B29,2)</f>
         <v>3</v>
@@ -1708,8 +1783,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="21"/>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="27"/>
       <c r="B31" s="15">
         <f t="shared" si="20"/>
         <v>1</v>
@@ -1730,8 +1805,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="21"/>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="27"/>
       <c r="B32" s="3"/>
       <c r="C32" s="4"/>
       <c r="D32" s="3">
@@ -1746,8 +1821,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="21"/>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="27"/>
       <c r="B33" s="3"/>
       <c r="C33" s="4"/>
       <c r="D33" s="3">
@@ -1762,8 +1837,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="21"/>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="27"/>
       <c r="B34" s="3"/>
       <c r="C34" s="4"/>
       <c r="D34" s="3">
@@ -1778,8 +1853,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="22"/>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="28"/>
       <c r="B35" s="5"/>
       <c r="C35" s="7"/>
       <c r="D35" s="5">
@@ -1794,8 +1869,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="20">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="26">
         <v>48.25</v>
       </c>
       <c r="B36" s="1">
@@ -1814,8 +1889,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="21"/>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="27"/>
       <c r="B37" s="3">
         <f>QUOTIENT(B36,2)</f>
         <v>24</v>
@@ -1836,8 +1911,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="21"/>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="27"/>
       <c r="B38" s="3">
         <f t="shared" ref="B38:B41" si="23">QUOTIENT(B37,2)</f>
         <v>12</v>
@@ -1849,8 +1924,8 @@
       <c r="D38" s="3"/>
       <c r="F38" s="9"/>
     </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="21"/>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="27"/>
       <c r="B39" s="3">
         <f t="shared" si="23"/>
         <v>6</v>
@@ -1862,8 +1937,8 @@
       <c r="D39" s="3"/>
       <c r="F39" s="9"/>
     </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="21"/>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="27"/>
       <c r="B40" s="3">
         <f t="shared" si="23"/>
         <v>3</v>
@@ -1875,8 +1950,8 @@
       <c r="D40" s="3"/>
       <c r="F40" s="9"/>
     </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="22"/>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="28"/>
       <c r="B41" s="11">
         <f t="shared" si="23"/>
         <v>1</v>
@@ -1889,8 +1964,8 @@
       <c r="E41" s="6"/>
       <c r="F41" s="10"/>
     </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="20">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="26">
         <v>23.125</v>
       </c>
       <c r="B42" s="1">
@@ -1909,8 +1984,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="21"/>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="27"/>
       <c r="B43" s="3">
         <f>QUOTIENT(B42,2)</f>
         <v>11</v>
@@ -1931,8 +2006,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="21"/>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="27"/>
       <c r="B44" s="3">
         <f>QUOTIENT(B43,2)</f>
         <v>5</v>
@@ -1953,8 +2028,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="21"/>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="27"/>
       <c r="B45" s="3">
         <f>QUOTIENT(B44,2)</f>
         <v>2</v>
@@ -1966,8 +2041,8 @@
       <c r="D45" s="3"/>
       <c r="F45" s="9"/>
     </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="22"/>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="28"/>
       <c r="B46" s="13">
         <f>QUOTIENT(B45,2)</f>
         <v>1</v>
@@ -1980,8 +2055,8 @@
       <c r="E46" s="6"/>
       <c r="F46" s="10"/>
     </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="20">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="26">
         <v>51.7</v>
       </c>
       <c r="B47" s="1">
@@ -2000,8 +2075,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
-      <c r="A48" s="21"/>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="27"/>
       <c r="B48" s="3">
         <f>QUOTIENT(B47,2)</f>
         <v>25</v>
@@ -2022,8 +2097,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="21"/>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="27"/>
       <c r="B49" s="3">
         <f>QUOTIENT(B48,2)</f>
         <v>12</v>
@@ -2044,8 +2119,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="21"/>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="27"/>
       <c r="B50" s="3">
         <f>QUOTIENT(B49,2)</f>
         <v>6</v>
@@ -2066,8 +2141,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="21"/>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="27"/>
       <c r="B51" s="3">
         <f>QUOTIENT(B50,2)</f>
         <v>3</v>
@@ -2088,8 +2163,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="21"/>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="27"/>
       <c r="B52" s="13">
         <f>QUOTIENT(B51,2)</f>
         <v>1</v>
@@ -2110,8 +2185,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="21"/>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="27"/>
       <c r="B53" s="3"/>
       <c r="C53" s="4"/>
       <c r="D53" s="3">
@@ -2126,8 +2201,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="21"/>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="27"/>
       <c r="B54" s="3"/>
       <c r="C54" s="4"/>
       <c r="D54" s="3">
@@ -2142,8 +2217,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="21"/>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="27"/>
       <c r="B55" s="3"/>
       <c r="C55" s="4"/>
       <c r="D55" s="3">
@@ -2158,8 +2233,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="22"/>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="28"/>
       <c r="B56" s="5"/>
       <c r="C56" s="7"/>
       <c r="D56" s="5">
@@ -2176,17 +2251,17 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A47:A56"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A36:A41"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A8:A28"/>
     <mergeCell ref="B1:C2"/>
     <mergeCell ref="D1:F2"/>
     <mergeCell ref="A42:A46"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="AC4:AC6"/>
     <mergeCell ref="AC7:AC8"/>
-    <mergeCell ref="A47:A56"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A36:A41"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="A8:A28"/>
     <mergeCell ref="I4:I8"/>
     <mergeCell ref="J4:J8"/>
   </mergeCells>
@@ -2202,161 +2277,991 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51FAEC6C-1B1D-4A7B-9F1F-975F14C39F83}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="17"/>
+      <c r="B1" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1">
+        <v>23</v>
+      </c>
+      <c r="I1">
+        <v>2</v>
+      </c>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="17">
+        <v>23</v>
+      </c>
+      <c r="B2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="C2" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>11</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="17">
+        <v>47</v>
+      </c>
+      <c r="B3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C3" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>5</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="17">
+        <v>-14</v>
+      </c>
+      <c r="B4" s="19">
+        <v>101110</v>
+      </c>
+      <c r="C4" s="19">
+        <v>110001</v>
+      </c>
+      <c r="D4" s="19">
+        <v>110010</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="17">
+        <v>-21</v>
+      </c>
+      <c r="B5" s="17">
+        <v>1010101</v>
+      </c>
+      <c r="C5" s="17">
+        <v>1101010</v>
+      </c>
+      <c r="D5" s="17">
+        <v>1101011</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="17">
+        <v>-27</v>
+      </c>
+      <c r="B6" s="17">
+        <v>1011011</v>
+      </c>
+      <c r="C6" s="17">
+        <v>1100100</v>
+      </c>
+      <c r="D6" s="17">
+        <v>1100101</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="17">
+        <v>213</v>
+      </c>
+      <c r="B7" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="17" t="s">
+      <c r="C7" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7">
+        <v>47</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>23</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>11</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>5</v>
+      </c>
+      <c r="L10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
+      </c>
+      <c r="M11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <v>14</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>7</v>
+      </c>
+      <c r="J15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>3</v>
+      </c>
+      <c r="K16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H19">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="32">
-        <v>23</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="33" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="32">
-        <v>47</v>
-      </c>
-      <c r="B3" s="33" t="s">
+      <c r="I19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
         <v>10</v>
       </c>
-      <c r="C3" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="33" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="32">
-        <v>-14</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="32" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="32">
-        <v>-21</v>
-      </c>
-      <c r="B5" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="32" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="32">
-        <v>-27</v>
-      </c>
-      <c r="B6" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="32" t="s">
+      <c r="J20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>5</v>
+      </c>
+      <c r="K21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>2</v>
+      </c>
+      <c r="L22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H25">
+        <v>27</v>
+      </c>
+      <c r="I25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>13</v>
+      </c>
+      <c r="J26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>6</v>
+      </c>
+      <c r="K27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>3</v>
+      </c>
+      <c r="L28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H31">
+        <v>213</v>
+      </c>
+      <c r="I31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>106</v>
+      </c>
+      <c r="J32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>53</v>
+      </c>
+      <c r="K33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="K34">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="32">
-        <v>213</v>
-      </c>
-      <c r="B7" s="32" t="s">
+      <c r="L34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
         <v>13</v>
       </c>
-      <c r="C7" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="32" t="s">
-        <v>27</v>
+      <c r="M35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36">
+        <v>6</v>
+      </c>
+      <c r="N36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="M37">
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <v>3</v>
+      </c>
+      <c r="O37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="N38">
+        <v>1</v>
+      </c>
+      <c r="O38">
+        <v>1</v>
+      </c>
+      <c r="P38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="O39">
+        <v>1</v>
+      </c>
+      <c r="P39">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="B6:C6 B2:C3 B7:C7 B4:C4 B5:C5 D7 D2 D3 D4 D5 D6 E2:E7" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493D1E45-CE79-430B-B487-A22C8C16D2D9}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="2" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32">
+        <v>117</v>
+      </c>
+      <c r="D1" s="32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>58</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>29</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>14</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>7</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10">
+        <v>123</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>61</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>30</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>15</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>7</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>3</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="33" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="33" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C54">
+        <v>122</v>
+      </c>
+      <c r="D54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>61</v>
+      </c>
+      <c r="E55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>51</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>30</v>
+      </c>
+      <c r="F56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>23</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>15</v>
+      </c>
+      <c r="G57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>52</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+      <c r="G58">
+        <v>7</v>
+      </c>
+      <c r="H58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>53</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59">
+        <v>3</v>
+      </c>
+      <c r="I59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>54</v>
+      </c>
+      <c r="H60">
+        <v>1</v>
+      </c>
+      <c r="I60">
+        <v>1</v>
+      </c>
+      <c r="J60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I61">
+        <v>1</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>